<commit_message>
A Little Change in SPs :wink:
</commit_message>
<xml_diff>
--- a/Stored Procedures/WebServices/04_تیر/SKerman_SPs/راهنمای وب سرویس‌ اطلاعات داشبورد جنوب کرمان14000503_بخش1.xlsx
+++ b/Stored Procedures/WebServices/04_تیر/SKerman_SPs/راهنمای وب سرویس‌ اطلاعات داشبورد جنوب کرمان14000503_بخش1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Stored Procedures\WebServices\04_تیر\SKerman_SPs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81679CF1-0768-4044-88C8-0D50069FF744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A79D70-4BD6-4B88-9834-395226CA377F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
   <si>
     <t>int</t>
   </si>
@@ -194,9 +194,6 @@
   </si>
   <si>
     <t>cntPrivateMPFeeder</t>
-  </si>
-  <si>
-    <t>????</t>
   </si>
   <si>
     <t xml:space="preserve">  ناحیه (امور)</t>
@@ -288,6 +285,28 @@
  "FromDate" : "1397/02/01",
  "ToDate" : "1400/02/01"
 }</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">راهنمای وب سرویس‌ اطلاعات داشبورد جنوب کرمان_بخش1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Mitra"/>
+        <charset val="178"/>
+      </rPr>
+      <t>تذرو افزار 14000503</t>
+    </r>
+  </si>
+  <si>
+    <t>DisTime</t>
+  </si>
+  <si>
+    <t>DisTime_Tozi</t>
   </si>
   <si>
     <t>{
@@ -319,27 +338,13 @@
             "FaultyFeederName": "102-",
             "SAIDI_Tamir": 792812.64,
             "SAIDI": 475211.47,
+            "DisTime": 1608958.72,
+            "DisTime_Tozi": 1559163.19,
             "Rate": 1042.49,
             "DisRate": 286812.2
         }
     ]
 }</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">راهنمای وب سرویس‌ اطلاعات داشبورد جنوب کرمان_بخش1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="B Mitra"/>
-        <charset val="178"/>
-      </rPr>
-      <t>تذرو افزار 14000503</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -429,7 +434,7 @@
       <charset val="178"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="8.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -771,6 +776,63 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -791,63 +853,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1261,8 +1266,8 @@
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,20 +1278,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
+      <c r="A1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1295,10 +1300,10 @@
       <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="30"/>
     </row>
     <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1307,10 +1312,10 @@
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="32"/>
     </row>
     <row r="5" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1327,12 +1332,12 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
     </row>
     <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1363,12 +1368,12 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1377,10 +1382,10 @@
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="21"/>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1389,10 +1394,10 @@
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="21"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
@@ -1401,10 +1406,10 @@
       <c r="B12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="42"/>
     </row>
     <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1414,7 +1419,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="16"/>
     </row>
@@ -1426,7 +1431,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="16"/>
     </row>
@@ -1438,7 +1443,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="16"/>
     </row>
@@ -1450,7 +1455,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="16"/>
     </row>
@@ -1462,7 +1467,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="16"/>
     </row>
@@ -1474,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" s="16"/>
     </row>
@@ -1486,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="16"/>
     </row>
@@ -1498,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" s="16"/>
     </row>
@@ -1510,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="16"/>
     </row>
@@ -1522,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="16"/>
     </row>
@@ -1534,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D23" s="16"/>
     </row>
@@ -1546,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24" s="16"/>
     </row>
@@ -1558,7 +1563,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" s="16"/>
     </row>
@@ -1570,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D26" s="16"/>
     </row>
@@ -1582,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="16"/>
     </row>
@@ -1594,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="16"/>
     </row>
@@ -1606,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" s="16"/>
     </row>
@@ -1618,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D30" s="16"/>
     </row>
@@ -1630,7 +1635,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D31" s="16"/>
     </row>
@@ -1642,7 +1647,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="16"/>
     </row>
@@ -1654,7 +1659,7 @@
         <v>30</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" s="16"/>
     </row>
@@ -1666,7 +1671,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" s="16"/>
     </row>
@@ -1678,31 +1683,31 @@
         <v>30</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" s="16"/>
     </row>
     <row r="36" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" s="16"/>
     </row>
     <row r="37" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D37" s="16"/>
     </row>
@@ -1714,7 +1719,7 @@
         <v>30</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38" s="16"/>
     </row>
@@ -1726,7 +1731,7 @@
         <v>30</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D39" s="16"/>
     </row>
@@ -1738,32 +1743,57 @@
         <v>30</v>
       </c>
       <c r="C40" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="16"/>
+    </row>
+    <row r="41" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="18"/>
+      <c r="C41" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="20"/>
+    </row>
+    <row r="42" spans="1:4" ht="405" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="16"/>
-    </row>
-    <row r="41" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="40"/>
-    </row>
-    <row r="42" spans="1:4" ht="405" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" s="42"/>
+      <c r="B42" s="22"/>
       <c r="C42" s="43" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D42" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A6:D6"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="C41:D41"/>
@@ -1779,32 +1809,7 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
little change in SKerman_dashboard1 :grin:
</commit_message>
<xml_diff>
--- a/Stored Procedures/WebServices/04_تیر/SKerman_SPs/راهنمای وب سرویس‌ اطلاعات داشبورد جنوب کرمان14000503_بخش1.xlsx
+++ b/Stored Procedures/WebServices/04_تیر/SKerman_SPs/راهنمای وب سرویس‌ اطلاعات داشبورد جنوب کرمان14000503_بخش1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Stored Procedures\WebServices\04_تیر\SKerman_SPs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A79D70-4BD6-4B88-9834-395226CA377F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D1456B-456D-49D7-8567-2A7AE38C55D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="وب سرویس ثبت حادثه" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'وب سرویس ثبت حادثه'!$A$1:$D$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'وب سرویس ثبت حادثه'!$A$1:$D$44</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t>int</t>
   </si>
@@ -248,9 +248,6 @@
   </si>
   <si>
     <t>تعداد کل قطعی های با برنامه از پست</t>
-  </si>
-  <si>
-    <t>پرخطا ترین فیدر براساس مجموع انرژی توزیع نشده</t>
   </si>
   <si>
     <t>نرخ</t>
@@ -336,6 +333,7 @@
             "cntPublicMPFeeder": 326,
             "cntPrivateMPFeeder": 71,
             "FaultyFeederName": "102-",
+            "FaultyFeederCode": "20322",
             "SAIDI_Tamir": 792812.64,
             "SAIDI": 475211.47,
             "DisTime": 1608958.72,
@@ -345,6 +343,15 @@
         }
     ]
 }</t>
+  </si>
+  <si>
+    <t>FaultyFeederCode</t>
+  </si>
+  <si>
+    <t>کد پرخطا ترین فیدر براساس مجموع انرژی توزیع نشده</t>
+  </si>
+  <si>
+    <t>نام پرخطا ترین فیدر براساس مجموع انرژی توزیع نشده</t>
   </si>
 </sst>
 </file>
@@ -434,7 +441,7 @@
       <charset val="178"/>
     </font>
     <font>
-      <sz val="8.5"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -776,6 +783,66 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -793,66 +860,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1264,10 +1271,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39:D39"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,20 +1285,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="A1" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
     </row>
     <row r="3" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1300,10 +1307,10 @@
       <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="30"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1312,10 +1319,10 @@
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1332,12 +1339,12 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
     </row>
     <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1368,12 +1375,12 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1382,10 +1389,10 @@
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="40"/>
+      <c r="D10" s="21"/>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1394,10 +1401,10 @@
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="40"/>
+      <c r="D11" s="21"/>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
@@ -1406,10 +1413,10 @@
       <c r="B12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="42"/>
+      <c r="D12" s="23"/>
     </row>
     <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1635,171 +1642,158 @@
         <v>1</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="16"/>
+    </row>
+    <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="16"/>
-    </row>
-    <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D33" s="16"/>
     </row>
     <row r="34" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>51</v>
+      <c r="A34" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D34" s="16"/>
     </row>
     <row r="35" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D35" s="16"/>
     </row>
     <row r="36" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D36" s="16"/>
     </row>
     <row r="37" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D37" s="16"/>
     </row>
     <row r="38" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="16"/>
+    </row>
+    <row r="39" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" s="16"/>
-    </row>
-    <row r="39" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D39" s="16"/>
     </row>
-    <row r="40" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>45</v>
+    <row r="40" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C40" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="16"/>
+    </row>
+    <row r="41" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="16"/>
+    </row>
+    <row r="42" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="38"/>
+      <c r="C42" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="40"/>
+    </row>
+    <row r="43" spans="1:4" ht="408.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="16"/>
-    </row>
-    <row r="41" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="20"/>
-    </row>
-    <row r="42" spans="1:4" ht="405" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="44"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:D6"/>
+  <mergeCells count="42">
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C19:D19"/>
@@ -1810,6 +1804,32 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C31:D31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
A little change in SKerman01_Manual :triumph:
</commit_message>
<xml_diff>
--- a/Stored Procedures/WebServices/04_تیر/SKerman_SPs/راهنمای وب سرویس‌ اطلاعات داشبورد جنوب کرمان14000503_بخش1.xlsx
+++ b/Stored Procedures/WebServices/04_تیر/SKerman_SPs/راهنمای وب سرویس‌ اطلاعات داشبورد جنوب کرمان14000503_بخش1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Stored Procedures\WebServices\04_تیر\SKerman_SPs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D1456B-456D-49D7-8567-2A7AE38C55D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11039EE5-D776-4682-8F14-1365821E4BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,79 +199,31 @@
     <t xml:space="preserve">  ناحیه (امور)</t>
   </si>
   <si>
-    <t>انرژی توزیع نشده با برنامه فشار متوسط</t>
-  </si>
-  <si>
-    <t>انرژی توزیع نشده بی برنامه فشار متوسط</t>
-  </si>
-  <si>
     <t>انرژی توزیع نشده با برنامه فشار ضعیف</t>
   </si>
   <si>
     <t>انرژی توزیع نشده بی برنامه فشار ضعیف</t>
   </si>
   <si>
-    <t>مدت زمان خاموشی با برنامه فشار متوسط</t>
-  </si>
-  <si>
-    <t>مدت زمان خاموشی بی برنامه فشار متوسط</t>
-  </si>
-  <si>
     <t>مدت زمان خاموشی با برنامه فشار ضعیف</t>
   </si>
   <si>
     <t>مدت زمان خاموشی بی برنامه فشار ضعیف</t>
   </si>
   <si>
-    <t>تعداد خاموشی با برنامه فشار متوسط</t>
-  </si>
-  <si>
-    <t>تعداد خاموشی بی برنامه فشار متوسط</t>
-  </si>
-  <si>
     <t>تعداد خاموشی با برنامه فشار ضعیف</t>
   </si>
   <si>
     <t>تعداد خاموشی بی برنامه فشار ضعیف</t>
   </si>
   <si>
-    <t>تغداد فیدرهای عمومی با بیش از 3 خطا (قطع از پست)</t>
-  </si>
-  <si>
     <t>تعداد فیدرهای عمومی</t>
   </si>
   <si>
     <t>تعداد فیدرهای اختصاصی</t>
   </si>
   <si>
-    <t>تعداد کل قطعی های بی برنامه از پست</t>
-  </si>
-  <si>
-    <t>تعداد کل قطعی های با برنامه از پست</t>
-  </si>
-  <si>
-    <t>نرخ</t>
-  </si>
-  <si>
-    <t>نرخ زمان خاموشی هر مشترک</t>
-  </si>
-  <si>
-    <t>با برنامه SAIDI</t>
-  </si>
-  <si>
-    <t>بی برنامه SAIDI</t>
-  </si>
-  <si>
-    <t>زمان خاموشی هر مشترک در روز به دقیقه (توزیع . فوق توزیع و بالاتر)</t>
-  </si>
-  <si>
     <t>زمان خاموشی هر مشترک در روز به دقیقه (توزیع)</t>
-  </si>
-  <si>
-    <t>درصد فیدرهای پرخطای عمومی</t>
-  </si>
-  <si>
-    <t>متوسط زمان رفع خاموشی بی برنامه فشار متوسط</t>
   </si>
   <si>
     <t>متوسط زمان رفع خاموشی بی برنامه فشار ضعیف</t>
@@ -348,17 +300,116 @@
     <t>FaultyFeederCode</t>
   </si>
   <si>
-    <t>کد پرخطا ترین فیدر براساس مجموع انرژی توزیع نشده</t>
-  </si>
-  <si>
-    <t>نام پرخطا ترین فیدر براساس مجموع انرژی توزیع نشده</t>
+    <r>
+      <t xml:space="preserve">زمان خاموشی هر مشترک در روز به دقیقه (توزیع . فوق توزیع و بالاتر) = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="B Mitra"/>
+        <charset val="178"/>
+      </rPr>
+      <t>SAIDI + SAIDI_Tamir</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">نرخ (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نرخ زمان خاموشی هر مشترک (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">با برنامه </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="B Mitra"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">SAIDI  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="B Mitra"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">(بدون فوق توزیع و بالاتر) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">بی برنامه </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="B Mitra"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">SAIDI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="B Mitra"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve"> (بدون فوق توزیع و بالاتر) </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">درصد فیدرهای پرخطای عمومی (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">متوسط زمان رفع خاموشی بی برنامه فشار متوسط (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">کد پرخطا ترین فیدر براساس مجموع انرژی توزیع نشده (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">نام پرخطا ترین فیدر براساس مجموع انرژی توزیع نشده (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">تعداد کل قطعی های با برنامه از پست (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">تغداد فیدرهای عمومی با بیش از 3 خطا (قطع از پست) (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">تعداد خاموشی بی برنامه فشار متوسط (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">تعداد خاموشی با برنامه فشار متوسط (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">مدت زمان خاموشی با برنامه فشار متوسط (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">مدت زمان خاموشی بی برنامه فشار متوسط (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">انرژی توزیع نشده بی برنامه فشار متوسط (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">انرژی توزیع نشده با برنامه فشار متوسط (بدون فوق توزیع و بالاتر) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">تعداد کل قطعی های بی برنامه از پست (بدون فوق توزیع و بالاتر) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +499,12 @@
       <charset val="178"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="B Mitra"/>
+      <charset val="178"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -783,6 +840,69 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -803,69 +923,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1273,8 +1330,8 @@
   </sheetPr>
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:D33"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,20 +1342,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
+      <c r="A1" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1307,10 +1364,10 @@
       <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="32"/>
     </row>
     <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1319,10 +1376,10 @@
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="34"/>
     </row>
     <row r="5" spans="1:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1339,12 +1396,12 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
     </row>
     <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1375,12 +1432,12 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1389,10 +1446,10 @@
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="21"/>
+      <c r="D10" s="42"/>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1401,10 +1458,10 @@
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="21"/>
+      <c r="D11" s="42"/>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
@@ -1413,10 +1470,10 @@
       <c r="B12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="44"/>
     </row>
     <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1438,7 +1495,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="D14" s="16"/>
     </row>
@@ -1450,7 +1507,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D15" s="16"/>
     </row>
@@ -1462,7 +1519,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" s="16"/>
     </row>
@@ -1474,7 +1531,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D17" s="16"/>
     </row>
@@ -1486,7 +1543,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="D18" s="16"/>
     </row>
@@ -1498,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="D19" s="16"/>
     </row>
@@ -1510,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D20" s="16"/>
     </row>
@@ -1522,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D21" s="16"/>
     </row>
@@ -1534,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="D22" s="16"/>
     </row>
@@ -1546,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="D23" s="16"/>
     </row>
@@ -1558,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D24" s="16"/>
     </row>
@@ -1570,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D25" s="16"/>
     </row>
@@ -1582,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D26" s="16"/>
     </row>
@@ -1594,7 +1651,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D27" s="16"/>
     </row>
@@ -1606,7 +1663,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D28" s="16"/>
     </row>
@@ -1618,7 +1675,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="D29" s="16"/>
     </row>
@@ -1630,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D30" s="16"/>
     </row>
@@ -1642,19 +1699,19 @@
         <v>1</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D32" s="16"/>
     </row>
@@ -1708,25 +1765,25 @@
     </row>
     <row r="37" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D37" s="16"/>
     </row>
     <row r="38" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D38" s="16"/>
     </row>
@@ -1738,7 +1795,7 @@
         <v>30</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D39" s="16"/>
     </row>
@@ -1750,7 +1807,7 @@
         <v>30</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D40" s="16"/>
     </row>
@@ -1762,32 +1819,58 @@
         <v>30</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D41" s="16"/>
     </row>
     <row r="42" spans="1:4" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="39" t="s">
+      <c r="B42" s="18"/>
+      <c r="C42" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="40"/>
+      <c r="D42" s="20"/>
     </row>
     <row r="43" spans="1:4" ht="408.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="42"/>
-      <c r="C43" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="44"/>
+      <c r="A43" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="22"/>
+      <c r="C43" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A6:D6"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="C42:D42"/>
@@ -1804,32 +1887,6 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C31:D31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>